<commit_message>
WIP: Added tests. Fixed bug where ALL matches were ignored due to refactoring.
</commit_message>
<xml_diff>
--- a/SearcherLibrary.Tests/FilesToTest/Excel.xlsx
+++ b/SearcherLibrary.Tests/FilesToTest/Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DJ\VS_Apps\VS_2019\Searcher\SearcherLibrary.Tests\FilesToTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B52AA-594E-4A2A-85CD-A91817A63681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E849E6B-CF8D-4617-AA5A-D56220B80070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="2085" windowWidth="25590" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>The quick</t>
   </si>
@@ -36,6 +36,9 @@
   <si>
     <t>over the 
 lazy dog</t>
+  </si>
+  <si>
+    <t>01/01/0002</t>
   </si>
 </sst>
 </file>
@@ -71,11 +74,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,7 +362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -381,20 +385,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2D20E5-22BC-42E7-B6B1-0FA462A487AD}">
-  <dimension ref="B2"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>